<commit_message>
-Updating Hardware Interfaces 2020.xlsx based on new PTO idea.
</commit_message>
<xml_diff>
--- a/Hardware Interfaces 2020.xlsx
+++ b/Hardware Interfaces 2020.xlsx
@@ -16,8 +16,68 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Luke Scime</author>
+  </authors>
+  <commentList>
+    <comment ref="G12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Luke Scime:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This is currently the intake and currently set to CAN ID 5
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Luke Scime:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+or ultrasonic range finder if lexan is transparent
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="175">
   <si>
     <t>PDP</t>
   </si>
@@ -337,15 +397,6 @@
     <t>LEDs w/ fuse</t>
   </si>
   <si>
-    <t>Winch</t>
-  </si>
-  <si>
-    <t>Level Climb</t>
-  </si>
-  <si>
-    <t>Intake 0/1</t>
-  </si>
-  <si>
     <t>Magazine/Spinner</t>
   </si>
   <si>
@@ -355,9 +406,6 @@
     <t>Intake Deploy</t>
   </si>
   <si>
-    <t>Clutch 0</t>
-  </si>
-  <si>
     <t>Hook Deploy</t>
   </si>
   <si>
@@ -373,18 +421,9 @@
     <t>LimeLight Tilt</t>
   </si>
   <si>
-    <t>?/IMU 1</t>
-  </si>
-  <si>
     <t>Beam Break</t>
   </si>
   <si>
-    <t>Index 0</t>
-  </si>
-  <si>
-    <t>Index 1</t>
-  </si>
-  <si>
     <t>RSL Light</t>
   </si>
   <si>
@@ -511,14 +550,65 @@
     <t>Toggle Intake</t>
   </si>
   <si>
-    <t>Intake/IMU 0</t>
+    <t>Intake/Level Climb</t>
+  </si>
+  <si>
+    <t>Boost/Winch</t>
+  </si>
+  <si>
+    <t>Turret</t>
+  </si>
+  <si>
+    <t>Spark Max - Neo</t>
+  </si>
+  <si>
+    <t>Victor SPX - Bag/Bag</t>
+  </si>
+  <si>
+    <t>Talon SRX - ?</t>
+  </si>
+  <si>
+    <t>Winch PTO</t>
+  </si>
+  <si>
+    <t>Talon FX - Falcon 500</t>
+  </si>
+  <si>
+    <t>Cowl 0</t>
+  </si>
+  <si>
+    <t>Cowl 1</t>
+  </si>
+  <si>
+    <t>Boost Index</t>
+  </si>
+  <si>
+    <t>Turret/IMU 0</t>
+  </si>
+  <si>
+    <t>Boost</t>
+  </si>
+  <si>
+    <t>Talon FX</t>
+  </si>
+  <si>
+    <t>Talon SPX</t>
+  </si>
+  <si>
+    <t>PCM 2</t>
+  </si>
+  <si>
+    <t>PCM 3</t>
+  </si>
+  <si>
+    <t>IR Range Finder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,8 +616,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,6 +667,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -741,7 +850,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -815,9 +924,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,6 +940,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF99"/>
       <color rgb="FFC9FFC9"/>
     </mruColors>
   </colors>
@@ -1127,14 +1242,14 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D13" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.109375" customWidth="1"/>
     <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1"/>
@@ -1201,7 +1316,7 @@
         <v>40</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>6</v>
@@ -1218,10 +1333,10 @@
         <v>0</v>
       </c>
       <c r="L3" s="35" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M3" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -1232,7 +1347,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="D4" s="36" t="s">
         <v>7</v>
@@ -1249,10 +1364,10 @@
         <v>1</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>112</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -1263,7 +1378,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="D5" s="36" t="s">
         <v>8</v>
@@ -1284,10 +1399,10 @@
         <v>2</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -1298,7 +1413,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>9</v>
@@ -1319,10 +1434,10 @@
         <v>3</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -1333,7 +1448,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="D7" s="36" t="s">
         <v>10</v>
@@ -1350,10 +1465,10 @@
         <v>4</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1364,7 +1479,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="D8" s="36" t="s">
         <v>11</v>
@@ -1381,10 +1496,10 @@
         <v>5</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1395,7 +1510,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="D9" s="36" t="s">
         <v>12</v>
@@ -1404,7 +1519,7 @@
         <v>27</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="H9" s="36" t="s">
         <v>19</v>
@@ -1416,10 +1531,10 @@
         <v>6</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>112</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1430,7 +1545,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>5</v>
+        <v>160</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>13</v>
@@ -1447,10 +1562,10 @@
         <v>7</v>
       </c>
       <c r="L10" s="35" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M10" s="36" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1512,9 +1627,11 @@
       <c r="B13" s="5">
         <v>30</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="21" t="s">
+        <v>161</v>
+      </c>
       <c r="D13" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="4">
@@ -1523,8 +1640,12 @@
       <c r="K13" s="29">
         <v>0</v>
       </c>
-      <c r="L13" s="6"/>
-      <c r="M13" s="7"/>
+      <c r="L13" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>165</v>
+      </c>
       <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1534,9 +1655,11 @@
       <c r="B14" s="5">
         <v>30</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="21" t="s">
+        <v>161</v>
+      </c>
       <c r="D14" s="7" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="4">
@@ -1545,8 +1668,12 @@
       <c r="K14" s="29">
         <v>1</v>
       </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="7"/>
+      <c r="L14" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>166</v>
+      </c>
       <c r="N14" s="6"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1556,9 +1683,11 @@
       <c r="B15" s="5">
         <v>40</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="21" t="s">
+        <v>162</v>
+      </c>
       <c r="D15" s="7" t="s">
-        <v>106</v>
+        <v>159</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="4">
@@ -1578,9 +1707,11 @@
       <c r="B16" s="5">
         <v>40</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>164</v>
+      </c>
       <c r="D16" s="7" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="4">
@@ -1594,15 +1725,17 @@
       <c r="N16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="48">
+      <c r="A17" s="51">
         <v>14</v>
       </c>
-      <c r="B17" s="51">
+      <c r="B17" s="29">
         <v>40</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="50" t="s">
-        <v>161</v>
+      <c r="C17" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="J17" s="4">
         <v>1</v>
@@ -1614,15 +1747,17 @@
       <c r="M17" s="7"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="48">
+      <c r="A18" s="51">
         <v>15</v>
       </c>
-      <c r="B18" s="51">
+      <c r="B18" s="29">
         <v>40</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="50" t="s">
-        <v>162</v>
+      <c r="C18" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>155</v>
       </c>
       <c r="J18" s="4">
         <v>1</v>
@@ -1652,8 +1787,12 @@
       <c r="K19" s="5">
         <v>6</v>
       </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="7"/>
+      <c r="L19" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
@@ -1674,8 +1813,12 @@
       <c r="K20" s="5">
         <v>7</v>
       </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="7"/>
+      <c r="L20" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="37">
@@ -1715,11 +1858,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1797,10 +1940,10 @@
         <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>90</v>
+        <v>167</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="33">
@@ -1831,11 +1974,11 @@
       <c r="A4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>119</v>
+      <c r="B4" t="s">
+        <v>89</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="33">
@@ -1866,12 +2009,8 @@
       <c r="A5" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>121</v>
-      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="7"/>
       <c r="D5" s="6"/>
       <c r="E5" s="33">
         <v>2</v>
@@ -1900,14 +2039,14 @@
       <c r="B6" s="21"/>
       <c r="C6" s="7"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="33">
-        <v>5</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>104</v>
-      </c>
-      <c r="G6" s="36" t="s">
-        <v>164</v>
+      <c r="E6" s="52">
+        <v>3</v>
+      </c>
+      <c r="F6" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>172</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>40</v>
@@ -1927,14 +2066,14 @@
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="4">
-        <v>6</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="G7" s="22" t="s">
-        <v>118</v>
+      <c r="E7" s="52">
+        <v>4</v>
+      </c>
+      <c r="F7" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="54" t="s">
+        <v>173</v>
       </c>
       <c r="I7" s="19" t="s">
         <v>41</v>
@@ -2046,14 +2185,14 @@
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="33">
-        <v>20</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="36" t="s">
-        <v>10</v>
+      <c r="E12" s="48">
+        <v>14</v>
+      </c>
+      <c r="F12" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="50" t="s">
+        <v>168</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>46</v>
@@ -2072,14 +2211,14 @@
         <v>75</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="33">
-        <v>21</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="36" t="s">
-        <v>11</v>
+      <c r="E13" s="4">
+        <v>15</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>169</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>82</v>
@@ -2098,14 +2237,14 @@
         <v>76</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="33">
-        <v>22</v>
-      </c>
-      <c r="F14" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>12</v>
+      <c r="E14" s="4">
+        <v>16</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>154</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>83</v>
@@ -2124,14 +2263,14 @@
         <v>77</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="33">
-        <v>23</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" s="36" t="s">
-        <v>13</v>
+      <c r="E15" s="51">
+        <v>17</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>155</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>84</v>
@@ -2150,14 +2289,14 @@
         <v>78</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="48">
-        <v>7</v>
-      </c>
-      <c r="F16" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="50" t="s">
-        <v>161</v>
+      <c r="E16" s="51">
+        <v>18</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>106</v>
       </c>
       <c r="I16" s="19" t="s">
         <v>85</v>
@@ -2170,20 +2309,20 @@
         <v>51</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="48">
-        <v>8</v>
-      </c>
-      <c r="F17" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="50" t="s">
-        <v>162</v>
+      <c r="E17" s="51">
+        <v>19</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>157</v>
       </c>
       <c r="I17" s="19" t="s">
         <v>86</v>
@@ -2202,9 +2341,15 @@
         <v>80</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
+      <c r="E18" s="33">
+        <v>20</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="36" t="s">
+        <v>10</v>
+      </c>
       <c r="I18" s="19" t="s">
         <v>87</v>
       </c>
@@ -2218,9 +2363,15 @@
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
+      <c r="E19" s="33">
+        <v>21</v>
+      </c>
+      <c r="F19" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="36" t="s">
+        <v>11</v>
+      </c>
       <c r="I19" s="19" t="s">
         <v>47</v>
       </c>
@@ -2228,7 +2379,7 @@
         <v>74</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2238,14 +2389,20 @@
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="E20" s="33">
+        <v>22</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="36" t="s">
+        <v>12</v>
+      </c>
       <c r="I20" s="19" t="s">
         <v>48</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>91</v>
@@ -2258,14 +2415,20 @@
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
+      <c r="E21" s="33">
+        <v>23</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>13</v>
+      </c>
       <c r="I21" s="19" t="s">
         <v>49</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>89</v>
+        <v>174</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>91</v>
@@ -2285,10 +2448,10 @@
         <v>50</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2432,7 +2595,7 @@
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="E34" s="5"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
     </row>
@@ -2441,13 +2604,13 @@
         <v>69</v>
       </c>
       <c r="B35" s="35" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C35" s="36" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="E35" s="5"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
@@ -2458,7 +2621,7 @@
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="E36" s="5"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
     </row>
@@ -2469,7 +2632,7 @@
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+      <c r="E37" s="5"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
     </row>
@@ -2523,8 +2686,29 @@
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
     </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2544,15 +2728,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2566,7 +2750,7 @@
         <v>102</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2574,7 +2758,7 @@
         <v>100</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2582,160 +2766,160 @@
         <v>101</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="41" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="41" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="41" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="47" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B11" s="22"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="47" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B12" s="22"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B14" s="7"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B15" s="7"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B17" s="11"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B18" s="11"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B19" s="11"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="36" t="s">
         <v>152</v>
-      </c>
-      <c r="B22" s="36" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B23" s="7"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B25" s="7"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="45" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B27" s="46"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="45" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B28" s="46"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="43" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B29" s="44"/>
     </row>
     <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="20" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B30" s="13"/>
     </row>

</xml_diff>

<commit_message>
updated can id for sparks
</commit_message>
<xml_diff>
--- a/Hardware Interfaces 2020.xlsx
+++ b/Hardware Interfaces 2020.xlsx
@@ -1862,7 +1862,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="51">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>170</v>

</xml_diff>

<commit_message>
-Updates the list of driver buttons being used
</commit_message>
<xml_diff>
--- a/Hardware Interfaces 2020.xlsx
+++ b/Hardware Interfaces 2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="48" windowWidth="11460" windowHeight="7704" activeTab="1"/>
+    <workbookView xWindow="96" yWindow="48" windowWidth="11460" windowHeight="7704" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Power Distribution" sheetId="1" r:id="rId1"/>
@@ -22,31 +22,6 @@
     <author>Luke Scime</author>
   </authors>
   <commentList>
-    <comment ref="G12" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Luke Scime:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-This is currently the intake and currently set to CAN ID 5
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="J20" authorId="0">
       <text>
         <r>
@@ -77,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="181">
   <si>
     <t>PDP</t>
   </si>
@@ -451,9 +426,6 @@
     <t xml:space="preserve">Rotate </t>
   </si>
   <si>
-    <t>Right Joystck Y</t>
-  </si>
-  <si>
     <t>Left Trigger</t>
   </si>
   <si>
@@ -550,9 +522,6 @@
     <t>Toggle Intake</t>
   </si>
   <si>
-    <t>Intake/Level Climb</t>
-  </si>
-  <si>
     <t>Boost/Winch</t>
   </si>
   <si>
@@ -583,9 +552,6 @@
     <t>Boost Index</t>
   </si>
   <si>
-    <t>Turret/IMU 0</t>
-  </si>
-  <si>
     <t>Boost</t>
   </si>
   <si>
@@ -602,6 +568,33 @@
   </si>
   <si>
     <t>Victor SPX</t>
+  </si>
+  <si>
+    <t>Turret/Winch/IMU 0</t>
+  </si>
+  <si>
+    <t>Intake</t>
+  </si>
+  <si>
+    <t>Victor SPX - ?</t>
+  </si>
+  <si>
+    <t>HP Signal</t>
+  </si>
+  <si>
+    <t>Emergency Boost</t>
+  </si>
+  <si>
+    <t>Right Joystick Y</t>
+  </si>
+  <si>
+    <t>Auto-Targeting</t>
+  </si>
+  <si>
+    <t>Fire Control Override</t>
+  </si>
+  <si>
+    <t>Defensive Pivot</t>
   </si>
 </sst>
 </file>
@@ -630,7 +623,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -663,12 +656,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -850,7 +837,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -914,24 +901,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,8 +922,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC9FFC9"/>
       <color rgb="FFFFFF99"/>
-      <color rgb="FFC9FFC9"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1242,7 +1224,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:D14"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1316,7 +1298,7 @@
         <v>40</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>6</v>
@@ -1347,7 +1329,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D4" s="36" t="s">
         <v>7</v>
@@ -1367,7 +1349,7 @@
         <v>107</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -1378,7 +1360,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D5" s="36" t="s">
         <v>8</v>
@@ -1413,7 +1395,7 @@
         <v>40</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>9</v>
@@ -1448,7 +1430,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D7" s="36" t="s">
         <v>10</v>
@@ -1479,7 +1461,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D8" s="36" t="s">
         <v>11</v>
@@ -1510,7 +1492,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D9" s="36" t="s">
         <v>12</v>
@@ -1534,7 +1516,7 @@
         <v>110</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1545,7 +1527,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>13</v>
@@ -1628,7 +1610,7 @@
         <v>30</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>106</v>
@@ -1644,7 +1626,7 @@
         <v>107</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="N13" s="6"/>
     </row>
@@ -1656,10 +1638,10 @@
         <v>30</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="4">
@@ -1672,7 +1654,7 @@
         <v>107</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="N14" s="6"/>
     </row>
@@ -1684,10 +1666,10 @@
         <v>40</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="4">
@@ -1708,10 +1690,10 @@
         <v>40</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="4">
@@ -1725,17 +1707,17 @@
       <c r="N16" s="6"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="51">
+      <c r="A17" s="46">
         <v>14</v>
       </c>
       <c r="B17" s="29">
         <v>40</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J17" s="4">
         <v>1</v>
@@ -1747,17 +1729,17 @@
       <c r="M17" s="7"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="51">
+      <c r="A18" s="46">
         <v>15</v>
       </c>
       <c r="B18" s="29">
         <v>40</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J18" s="4">
         <v>1</v>
@@ -1791,7 +1773,7 @@
         <v>110</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1817,7 +1799,7 @@
         <v>110</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1861,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1871,7 +1853,8 @@
     <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="1.77734375" customWidth="1"/>
-    <col min="5" max="7" width="16.88671875" customWidth="1"/>
+    <col min="5" max="6" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.21875" customWidth="1"/>
     <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.44140625" bestFit="1" customWidth="1"/>
@@ -1943,7 +1926,7 @@
         <v>114</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="33">
@@ -2039,14 +2022,14 @@
       <c r="B6" s="21"/>
       <c r="C6" s="7"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="52">
+      <c r="E6" s="47">
         <v>3</v>
       </c>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="54" t="s">
-        <v>171</v>
+      <c r="G6" s="49" t="s">
+        <v>168</v>
       </c>
       <c r="I6" s="19" t="s">
         <v>40</v>
@@ -2066,14 +2049,14 @@
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="52">
+      <c r="E7" s="47">
         <v>4</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="54" t="s">
-        <v>172</v>
+      <c r="G7" s="49" t="s">
+        <v>169</v>
       </c>
       <c r="I7" s="19" t="s">
         <v>41</v>
@@ -2185,14 +2168,14 @@
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="48">
+      <c r="E12" s="46">
         <v>14</v>
       </c>
-      <c r="F12" s="49" t="s">
+      <c r="F12" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="G12" s="50" t="s">
-        <v>168</v>
+      <c r="G12" s="22" t="s">
+        <v>172</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>46</v>
@@ -2215,10 +2198,10 @@
         <v>15</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>82</v>
@@ -2241,10 +2224,10 @@
         <v>16</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>83</v>
@@ -2263,14 +2246,14 @@
         <v>77</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="51">
+      <c r="E15" s="46">
         <v>17</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>84</v>
@@ -2289,11 +2272,11 @@
         <v>78</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="51">
+      <c r="E16" s="46">
         <v>18</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>106</v>
@@ -2315,14 +2298,14 @@
         <v>113</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="51">
+      <c r="E17" s="46">
         <v>19</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="I17" s="19" t="s">
         <v>86</v>
@@ -2379,7 +2362,7 @@
         <v>74</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2402,7 +2385,7 @@
         <v>48</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>91</v>
@@ -2428,7 +2411,7 @@
         <v>49</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>91</v>
@@ -2448,10 +2431,10 @@
         <v>50</v>
       </c>
       <c r="J22" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="K22" s="7" t="s">
         <v>150</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2716,8 +2699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2728,12 +2711,12 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>117</v>
@@ -2743,30 +2726,32 @@
       <c r="A3" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2795,133 +2780,145 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="11"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="11"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="B11" s="22"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="B12" s="22"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="B13" s="36" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="B13" s="7"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="36" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" s="7"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B17" s="11"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B18" s="11"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B19" s="11"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B23" s="7"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B25" s="7"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="B26" s="7"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="45" t="s">
+      <c r="B27" s="44"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="B27" s="46"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="45" t="s">
+      <c r="B28" s="44"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="B28" s="46"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="43" t="s">
+      <c r="B29" s="51" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="42" t="s">
         <v>142</v>
       </c>
-      <c r="B29" s="44"/>
-    </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="B30" s="13"/>
+      <c r="B30" s="40" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
-Updating for beta rebuild
</commit_message>
<xml_diff>
--- a/Hardware Interfaces 2020.xlsx
+++ b/Hardware Interfaces 2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Programming Projects\2020-Critical-Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2014ED-8F2D-4C3B-AC82-CF97178427D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E170C05-4FFE-41F2-88F3-9AC6AE67EBB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Distribution" sheetId="1" r:id="rId1"/>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1696,7 +1696,7 @@
         <v>145</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J17" s="29">
         <v>1</v>
@@ -1722,7 +1722,7 @@
         <v>145</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J18" s="29">
         <v>1</v>
@@ -1830,7 +1830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>